<commit_message>
Added Sounds + fixes
Added Sounds to multiple prefab actions + fixes
</commit_message>
<xml_diff>
--- a/C61/Sprint 3/Sprint3.xlsx
+++ b/C61/Sprint 3/Sprint3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\ProjetFinalC61\C61\Sprint 3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F31CF0CB-4C70-4C0A-A2D1-48518B5D748C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF80FD34-BE5B-476A-A94A-815FE20D9F2B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9F0BC983-5966-41D1-8204-26073EDFF06D}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="51">
   <si>
     <t>Tâche</t>
   </si>
@@ -160,6 +160,33 @@
   </si>
   <si>
     <t>Sanity System n'a pas été implémenté, non pertinent avec platformer</t>
+  </si>
+  <si>
+    <t>Usable class and prefabs</t>
+  </si>
+  <si>
+    <t>DialogManager</t>
+  </si>
+  <si>
+    <t>1,6,27</t>
+  </si>
+  <si>
+    <t>REPOUSSÉ DU SPRINT 2</t>
+  </si>
+  <si>
+    <t>Oui</t>
+  </si>
+  <si>
+    <t>Plus long que prévu, surtout à cause du UI/animation du menu/afficher les items correctement</t>
+  </si>
+  <si>
+    <t>Plus tous les ajouts (SaveLoadManager, Health/Mana bar UI, interaction prompt, etc)</t>
+  </si>
+  <si>
+    <t>100%</t>
+  </si>
+  <si>
+    <t>Inventory Menu/Manager</t>
   </si>
 </sst>
 </file>
@@ -252,7 +279,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -295,8 +322,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="17">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -458,36 +491,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -505,30 +508,100 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -566,12 +639,6 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -582,10 +649,7 @@
     <xf numFmtId="49" fontId="9" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -594,15 +658,8 @@
     <xf numFmtId="0" fontId="10" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -622,23 +679,104 @@
     <xf numFmtId="49" fontId="9" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="4" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -953,18 +1091,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50F59768-3BEF-4D94-98E2-7178D1BD8A0F}">
-  <dimension ref="A1:M18"/>
+  <dimension ref="A1:M21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="41" customWidth="1"/>
+    <col min="2" max="2" width="51.85546875" customWidth="1"/>
     <col min="3" max="3" width="14" customWidth="1"/>
     <col min="4" max="4" width="16.7109375" customWidth="1"/>
-    <col min="10" max="10" width="95.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="82.42578125" customWidth="1"/>
     <col min="11" max="11" width="7.140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -987,7 +1125,7 @@
       <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="22" t="s">
+      <c r="G1" s="19" t="s">
         <v>6</v>
       </c>
       <c r="H1" s="4" t="s">
@@ -999,145 +1137,145 @@
       <c r="J1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="16" t="s">
+      <c r="L1" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="M1" s="16" t="s">
+      <c r="M1" s="14" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="26">
+      <c r="A2" s="22">
         <v>33</v>
       </c>
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="30">
+      <c r="C2" s="24">
         <v>13</v>
       </c>
-      <c r="D2" s="31" t="s">
+      <c r="D2" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="31" t="s">
+      <c r="E2" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="31">
+      <c r="F2" s="25">
         <v>45</v>
       </c>
-      <c r="G2" s="32">
+      <c r="G2" s="26">
         <v>0</v>
       </c>
-      <c r="H2" s="37" t="s">
+      <c r="H2" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="I2" s="38" t="s">
+      <c r="I2" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="J2" s="39" t="s">
+      <c r="J2" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="L2" s="17" t="s">
+      <c r="L2" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="M2" s="18">
+      <c r="M2" s="16">
         <v>1515</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="26">
+      <c r="A3" s="22">
         <v>34</v>
       </c>
-      <c r="B3" s="29" t="s">
+      <c r="B3" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="30"/>
-      <c r="D3" s="31" t="s">
+      <c r="C3" s="24"/>
+      <c r="D3" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="31" t="s">
+      <c r="E3" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="31">
+      <c r="F3" s="25">
         <v>45</v>
       </c>
-      <c r="G3" s="32">
+      <c r="G3" s="26">
         <v>0</v>
       </c>
-      <c r="H3" s="33" t="s">
+      <c r="H3" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="I3" s="34" t="s">
+      <c r="I3" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="J3" s="35" t="s">
+      <c r="J3" s="32" t="s">
         <v>38</v>
       </c>
-      <c r="L3" s="17" t="s">
+      <c r="L3" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="M3" s="18">
+      <c r="M3" s="16">
         <f>SUM(G2:G13)</f>
         <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="26">
+      <c r="A4" s="22">
         <v>35</v>
       </c>
-      <c r="B4" s="29" t="s">
+      <c r="B4" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="30">
+      <c r="C4" s="24">
         <v>1</v>
       </c>
-      <c r="D4" s="31" t="s">
+      <c r="D4" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="31" t="s">
+      <c r="E4" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="31">
+      <c r="F4" s="25">
         <v>90</v>
       </c>
-      <c r="G4" s="32">
+      <c r="G4" s="26">
         <v>0</v>
       </c>
-      <c r="H4" s="33" t="s">
+      <c r="H4" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="I4" s="34" t="s">
+      <c r="I4" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="J4" s="40"/>
+      <c r="J4" s="33"/>
     </row>
     <row r="5" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="26">
+      <c r="A5" s="22">
         <v>36</v>
       </c>
-      <c r="B5" s="29" t="s">
+      <c r="B5" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="30"/>
-      <c r="D5" s="31" t="s">
+      <c r="C5" s="24"/>
+      <c r="D5" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="31" t="s">
+      <c r="E5" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="31">
+      <c r="F5" s="25">
         <v>45</v>
       </c>
-      <c r="G5" s="32">
+      <c r="G5" s="26">
         <v>0</v>
       </c>
-      <c r="H5" s="33" t="s">
+      <c r="H5" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="I5" s="34" t="s">
+      <c r="I5" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="J5" s="36"/>
+      <c r="J5" s="34"/>
     </row>
     <row r="6" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
@@ -1158,14 +1296,14 @@
       <c r="F6" s="10">
         <v>60</v>
       </c>
-      <c r="G6" s="23">
+      <c r="G6" s="20">
         <v>45</v>
       </c>
       <c r="H6" s="13"/>
-      <c r="I6" s="20" t="s">
+      <c r="I6" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="J6" s="19" t="s">
+      <c r="J6" s="17" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1188,72 +1326,72 @@
       <c r="F7" s="10">
         <v>240</v>
       </c>
-      <c r="G7" s="23"/>
+      <c r="G7" s="20"/>
       <c r="H7" s="13"/>
-      <c r="I7" s="20"/>
-      <c r="J7" s="19"/>
+      <c r="I7" s="18"/>
+      <c r="J7" s="17"/>
     </row>
     <row r="8" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="26">
+      <c r="A8" s="22">
         <v>39</v>
       </c>
-      <c r="B8" s="29" t="s">
+      <c r="B8" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="30" t="s">
+      <c r="C8" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="31" t="s">
+      <c r="D8" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="E8" s="31" t="s">
+      <c r="E8" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="F8" s="31">
+      <c r="F8" s="25">
         <v>60</v>
       </c>
-      <c r="G8" s="32">
+      <c r="G8" s="26">
         <v>0</v>
       </c>
-      <c r="H8" s="33" t="s">
+      <c r="H8" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="I8" s="34" t="s">
+      <c r="I8" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="J8" s="35" t="s">
+      <c r="J8" s="32" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="26">
+      <c r="A9" s="22">
         <v>40</v>
       </c>
-      <c r="B9" s="29" t="s">
+      <c r="B9" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="30" t="s">
+      <c r="C9" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="D9" s="31" t="s">
+      <c r="D9" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="E9" s="31" t="s">
+      <c r="E9" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="F9" s="31">
+      <c r="F9" s="25">
         <v>180</v>
       </c>
-      <c r="G9" s="32">
+      <c r="G9" s="26">
         <v>0</v>
       </c>
-      <c r="H9" s="33" t="s">
+      <c r="H9" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="I9" s="34" t="s">
+      <c r="I9" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="J9" s="36"/>
+      <c r="J9" s="34"/>
     </row>
     <row r="10" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
@@ -1274,40 +1412,40 @@
       <c r="F10" s="10">
         <v>90</v>
       </c>
-      <c r="G10" s="23"/>
+      <c r="G10" s="20"/>
       <c r="H10" s="13"/>
-      <c r="I10" s="20"/>
-      <c r="J10" s="19"/>
+      <c r="I10" s="18"/>
+      <c r="J10" s="17"/>
     </row>
     <row r="11" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="7">
         <v>42</v>
       </c>
-      <c r="B11" s="41" t="s">
+      <c r="B11" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="C11" s="27">
+      <c r="C11" s="24">
         <v>21</v>
       </c>
-      <c r="D11" s="28" t="s">
+      <c r="D11" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="E11" s="28" t="s">
+      <c r="E11" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="F11" s="28">
+      <c r="F11" s="25">
         <v>180</v>
       </c>
-      <c r="G11" s="23">
+      <c r="G11" s="26">
         <v>0</v>
       </c>
-      <c r="H11" s="13" t="s">
+      <c r="H11" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="I11" s="20" t="s">
+      <c r="I11" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="J11" s="24" t="s">
+      <c r="J11" s="47" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1328,10 +1466,10 @@
       <c r="F12" s="10">
         <v>240</v>
       </c>
-      <c r="G12" s="23"/>
+      <c r="G12" s="20"/>
       <c r="H12" s="13"/>
-      <c r="I12" s="20"/>
-      <c r="J12" s="24"/>
+      <c r="I12" s="18"/>
+      <c r="J12" s="21"/>
     </row>
     <row r="13" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="7">
@@ -1350,10 +1488,10 @@
       <c r="F13" s="10">
         <v>240</v>
       </c>
-      <c r="G13" s="23"/>
+      <c r="G13" s="20"/>
       <c r="H13" s="13"/>
-      <c r="I13" s="20"/>
-      <c r="J13" s="24"/>
+      <c r="I13" s="18"/>
+      <c r="J13" s="21"/>
     </row>
     <row r="14" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="7"/>
@@ -1362,65 +1500,154 @@
       <c r="D14" s="10"/>
       <c r="E14" s="10"/>
       <c r="F14" s="10"/>
-      <c r="G14" s="23"/>
+      <c r="G14" s="20"/>
       <c r="H14" s="13"/>
-      <c r="I14" s="20"/>
-      <c r="J14" s="24"/>
+      <c r="I14" s="18"/>
+      <c r="J14" s="21"/>
     </row>
     <row r="15" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="7"/>
-      <c r="B15" s="12"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="10"/>
-      <c r="G15" s="23"/>
-      <c r="H15" s="13"/>
-      <c r="I15" s="20"/>
-      <c r="J15" s="24"/>
-    </row>
-    <row r="16" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="6">
+      <c r="B15" s="35" t="s">
         <v>45</v>
       </c>
-      <c r="B16" s="12"/>
-      <c r="C16" s="9"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="10"/>
-      <c r="F16" s="10"/>
-      <c r="G16" s="15"/>
-      <c r="H16" s="13"/>
-      <c r="I16" s="20"/>
-      <c r="J16" s="24"/>
+      <c r="C15" s="36"/>
+      <c r="D15" s="37"/>
+      <c r="E15" s="37"/>
+      <c r="F15" s="37"/>
+      <c r="G15" s="38"/>
+      <c r="H15" s="39"/>
+      <c r="I15" s="40"/>
+      <c r="J15" s="41"/>
+    </row>
+    <row r="16" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="7"/>
+      <c r="B16" s="36" t="s">
+        <v>50</v>
+      </c>
+      <c r="C16" s="42">
+        <v>2</v>
+      </c>
+      <c r="D16" s="37" t="s">
+        <v>10</v>
+      </c>
+      <c r="E16" s="37" t="s">
+        <v>14</v>
+      </c>
+      <c r="F16" s="37">
+        <v>120</v>
+      </c>
+      <c r="G16" s="38">
+        <v>240</v>
+      </c>
+      <c r="H16" s="39" t="s">
+        <v>46</v>
+      </c>
+      <c r="I16" s="40"/>
+      <c r="J16" s="41" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="17" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="6"/>
-      <c r="B17" s="8"/>
-      <c r="C17" s="9"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="10"/>
-      <c r="G17" s="15"/>
-      <c r="H17" s="13"/>
-      <c r="I17" s="20"/>
-      <c r="J17" s="19"/>
-    </row>
-    <row r="18" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="43" t="s">
+        <v>42</v>
+      </c>
+      <c r="C17" s="42">
+        <v>2</v>
+      </c>
+      <c r="D17" s="37" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="F17" s="37">
+        <v>120</v>
+      </c>
+      <c r="G17" s="44">
+        <v>120</v>
+      </c>
+      <c r="H17" s="39" t="s">
+        <v>46</v>
+      </c>
+      <c r="I17" s="40" t="s">
+        <v>49</v>
+      </c>
+      <c r="J17" s="41"/>
+    </row>
+    <row r="18" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="6"/>
-      <c r="B18" s="12"/>
-      <c r="C18" s="9"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="10"/>
-      <c r="F18" s="10"/>
-      <c r="G18" s="15"/>
-      <c r="H18" s="14"/>
-      <c r="I18" s="21"/>
-      <c r="J18" s="25"/>
+      <c r="B18" s="36" t="s">
+        <v>43</v>
+      </c>
+      <c r="C18" s="42" t="s">
+        <v>44</v>
+      </c>
+      <c r="D18" s="37" t="s">
+        <v>16</v>
+      </c>
+      <c r="E18" s="37" t="s">
+        <v>14</v>
+      </c>
+      <c r="F18" s="37">
+        <v>240</v>
+      </c>
+      <c r="G18" s="44"/>
+      <c r="H18" s="39"/>
+      <c r="I18" s="40"/>
+      <c r="J18" s="45"/>
+    </row>
+    <row r="19" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="6"/>
+      <c r="B19" s="36"/>
+      <c r="C19" s="42"/>
+      <c r="D19" s="37"/>
+      <c r="E19" s="37"/>
+      <c r="F19" s="37"/>
+      <c r="G19" s="44"/>
+      <c r="H19" s="48"/>
+      <c r="I19" s="49"/>
+      <c r="J19" s="50"/>
+    </row>
+    <row r="20" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="6"/>
+      <c r="B20" s="51" t="s">
+        <v>48</v>
+      </c>
+      <c r="C20" s="53"/>
+      <c r="D20" s="55"/>
+      <c r="E20" s="55"/>
+      <c r="F20" s="55"/>
+      <c r="G20" s="57"/>
+      <c r="H20" s="59"/>
+      <c r="I20" s="61"/>
+      <c r="J20" s="63"/>
+    </row>
+    <row r="21" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="6"/>
+      <c r="B21" s="52"/>
+      <c r="C21" s="54"/>
+      <c r="D21" s="56"/>
+      <c r="E21" s="56"/>
+      <c r="F21" s="56"/>
+      <c r="G21" s="58"/>
+      <c r="H21" s="60"/>
+      <c r="I21" s="62"/>
+      <c r="J21" s="64"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="11">
     <mergeCell ref="J3:J5"/>
     <mergeCell ref="J8:J9"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="G20:G21"/>
+    <mergeCell ref="H20:H21"/>
+    <mergeCell ref="I20:I21"/>
+    <mergeCell ref="J20:J21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>